<commit_message>
Alteração da planilha de horarios
</commit_message>
<xml_diff>
--- a/Tabela_horario_atividades.xlsx
+++ b/Tabela_horario_atividades.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Master\Desktop\Gui\UEA_2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ThinkTEd\Desktop\Guib\UEA\uea_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDBD3AA-ED2A-48F7-86CD-2657ED799EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185BA248-394D-4DAA-B18B-E7A5A0DFED09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{703B2EFC-4204-4C7B-9AED-4B28892F0771}"/>
+    <workbookView xWindow="570" yWindow="1680" windowWidth="18900" windowHeight="11070" xr2:uid="{703B2EFC-4204-4C7B-9AED-4B28892F0771}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="27">
   <si>
     <t>Horarios</t>
   </si>
@@ -106,6 +107,12 @@
   </si>
   <si>
     <t xml:space="preserve">ThinkTEd </t>
+  </si>
+  <si>
+    <t>12:00 - 12:30</t>
+  </si>
+  <si>
+    <t>Proj. PD</t>
   </si>
 </sst>
 </file>
@@ -127,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +183,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -237,11 +250,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -268,9 +290,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -279,6 +298,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,63 +619,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A55AB79-15A5-4931-BE84-D7F5C1988CDC}">
-  <dimension ref="B1:H12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="C2" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
@@ -663,15 +690,15 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
@@ -684,17 +711,17 @@
       <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
@@ -707,136 +734,133 @@
       <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="12"/>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -846,11 +870,271 @@
       <c r="H12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="C6:H6"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6914BC2C-CCC7-4BD7-966C-1B5383B373F7}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modificação da tabela de atividades
</commit_message>
<xml_diff>
--- a/Tabela_horario_atividades.xlsx
+++ b/Tabela_horario_atividades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Master\Desktop\Gui\UEA_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDBD3AA-ED2A-48F7-86CD-2657ED799EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958D3C55-D303-44E5-A5EA-394C3A547771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{703B2EFC-4204-4C7B-9AED-4B28892F0771}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="8850" xr2:uid="{703B2EFC-4204-4C7B-9AED-4B28892F0771}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,8 +769,8 @@
       <c r="G8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>24</v>
+      <c r="H8" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -792,8 +792,8 @@
       <c r="G9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>24</v>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -815,8 +815,8 @@
       <c r="G10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>24</v>
+      <c r="H10" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>